<commit_message>
Road traffic index 2023.
</commit_message>
<xml_diff>
--- a/data_indexpoints_tidy/tallmateriale_952.xlsx
+++ b/data_indexpoints_tidy/tallmateriale_952.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Programmering\R\byindeks\data_indexpoints_tidy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E961C2B-D791-416D-9272-4E73995F6391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DC4D41-962D-4188-A50B-B6F9E1E45910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="punkt_adt" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,10 @@
     <sheet name="by_2_aar_glid_indeks" sheetId="6" r:id="rId6"/>
     <sheet name="by_1_aar_glid_indeks" sheetId="7" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">by_3_aar_glid_indeks!$A$1:$M$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">punkt_3_aar_glid_indeks!$A$1:$J$586</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -1068,9 +1072,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1108,9 +1112,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1143,26 +1147,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1195,26 +1182,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -40921,11 +40891,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J586"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -59681,6 +59662,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J586" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -59689,11 +59671,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="20.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -61255,6 +61251,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M38" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -63329,7 +63326,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Statistical distance metrics for historical index months, WIP
</commit_message>
<xml_diff>
--- a/data_indexpoints_tidy/tallmateriale_952.xlsx
+++ b/data_indexpoints_tidy/tallmateriale_952.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Programmering\R\byindeks\data_indexpoints_tidy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349241A5-219A-4124-A98F-5BCB12CF4E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7B8DC4-EAE4-4499-9268-9FC2FE9B3DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="punkt_adt" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,10 @@
     <sheet name="punkt_3_aar_glid_indeks" sheetId="5" r:id="rId5"/>
     <sheet name="by_glid_indeks" sheetId="6" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">by_glid_indeks!$A$1:$M$184</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">punkt_3_aar_glid_indeks!$A$1:$J$771</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -1517,7 +1521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -54215,11 +54219,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J771"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -78895,19 +78910,35 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J771" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:M184"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F143" sqref="F143"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="20.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -78951,7 +78982,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.9926191495103478</v>
       </c>
@@ -78992,7 +79023,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.99035669665966386</v>
       </c>
@@ -79033,7 +79064,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.98932397351401913</v>
       </c>
@@ -79074,7 +79105,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.99179003937932475</v>
       </c>
@@ -79115,7 +79146,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.98296872276124991</v>
       </c>
@@ -79156,7 +79187,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.98178696788075992</v>
       </c>
@@ -79197,7 +79228,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.9769813952909121</v>
       </c>
@@ -79238,7 +79269,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.97611933497008097</v>
       </c>
@@ -79279,7 +79310,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.97392964777468172</v>
       </c>
@@ -79320,7 +79351,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.97466224590049533</v>
       </c>
@@ -79361,7 +79392,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.97752005789619734</v>
       </c>
@@ -79402,7 +79433,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.97971618770675173</v>
       </c>
@@ -79443,7 +79474,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.98091640276879333</v>
       </c>
@@ -79484,7 +79515,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.98249031478159399</v>
       </c>
@@ -79525,7 +79556,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.98346625809703969</v>
       </c>
@@ -79566,7 +79597,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0.96424231833382001</v>
       </c>
@@ -79607,7 +79638,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0.94660420874752405</v>
       </c>
@@ -79648,7 +79679,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.93539765202260239</v>
       </c>
@@ -79689,7 +79720,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0.93777432500330149</v>
       </c>
@@ -79730,7 +79761,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0.94366689346558963</v>
       </c>
@@ -79771,7 +79802,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0.94265169467600352</v>
       </c>
@@ -79812,7 +79843,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.94144825325203141</v>
       </c>
@@ -79853,7 +79884,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.93811116055840704</v>
       </c>
@@ -79894,7 +79925,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0.94260782939214893</v>
       </c>
@@ -79935,7 +79966,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0.94015969917488995</v>
       </c>
@@ -79976,7 +80007,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0.9253447611868143</v>
       </c>
@@ -80017,7 +80048,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0.9193026092184412</v>
       </c>
@@ -80058,7 +80089,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0.93701247280307154</v>
       </c>
@@ -80099,7 +80130,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0.94717600155156234</v>
       </c>
@@ -80140,7 +80171,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0.95184381976828425</v>
       </c>
@@ -80181,7 +80212,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0.95432705145769481</v>
       </c>
@@ -80222,7 +80253,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0.95289332800397308</v>
       </c>
@@ -80263,7 +80294,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0.9544984749141181</v>
       </c>
@@ -80304,7 +80335,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0.94751900726894878</v>
       </c>
@@ -80345,7 +80376,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0.9492780979654557</v>
       </c>
@@ -80386,7 +80417,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0.95874684245248065</v>
       </c>
@@ -80427,7 +80458,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0.96005583419870943</v>
       </c>
@@ -80468,7 +80499,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>0.96588726059734131</v>
       </c>
@@ -80509,7 +80540,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0.96768026650166572</v>
       </c>
@@ -80550,7 +80581,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0.97576206410283362</v>
       </c>
@@ -80591,7 +80622,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0.98338431650141012</v>
       </c>
@@ -80632,7 +80663,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0.99333193006962239</v>
       </c>
@@ -80673,7 +80704,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>0.99369645782625693</v>
       </c>
@@ -80714,7 +80745,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>0.98875402407521584</v>
       </c>
@@ -80755,7 +80786,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>0.98899706770821949</v>
       </c>
@@ -80796,7 +80827,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>0.98792857532619383</v>
       </c>
@@ -80837,7 +80868,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>0.99241802924607625</v>
       </c>
@@ -80878,7 +80909,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>0.99363700438127489</v>
       </c>
@@ -80919,7 +80950,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>0.99518492522671198</v>
       </c>
@@ -80960,7 +80991,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1.002215909178211</v>
       </c>
@@ -81001,7 +81032,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1.008575007890856</v>
       </c>
@@ -81042,7 +81073,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1.0102537033782779</v>
       </c>
@@ -81083,7 +81114,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1.020346592901082</v>
       </c>
@@ -81124,7 +81155,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1.019286901353309</v>
       </c>
@@ -81165,7 +81196,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1.023757120393715</v>
       </c>
@@ -81206,7 +81237,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1.0276063486171709</v>
       </c>
@@ -81247,7 +81278,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1.031005501105174</v>
       </c>
@@ -81288,7 +81319,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1.032733836240185</v>
       </c>
@@ -81329,7 +81360,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1.035904410030285</v>
       </c>
@@ -81370,7 +81401,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1.037504999375235</v>
       </c>
@@ -81411,7 +81442,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1.0381428728233839</v>
       </c>
@@ -81452,7 +81483,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1.037265265592936</v>
       </c>
@@ -81493,7 +81524,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1.0365540121370591</v>
       </c>
@@ -81534,7 +81565,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1.0308311994395809</v>
       </c>
@@ -81575,7 +81606,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1.0425172485379319</v>
       </c>
@@ -81616,7 +81647,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1.0449882699339359</v>
       </c>
@@ -81657,7 +81688,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1.0424770957456539</v>
       </c>
@@ -81698,7 +81729,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1.045051354957202</v>
       </c>
@@ -81739,7 +81770,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1.046398971830419</v>
       </c>
@@ -81780,7 +81811,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1.0472213665747021</v>
       </c>
@@ -81821,7 +81852,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1.0497071026300191</v>
       </c>
@@ -81862,7 +81893,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1.050485227990372</v>
       </c>
@@ -81903,7 +81934,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1.0520339469660409</v>
       </c>
@@ -81944,7 +81975,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>0.98796092760701082</v>
       </c>
@@ -81985,7 +82016,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>0.9874850176692227</v>
       </c>
@@ -82026,7 +82057,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>0.98745435958793359</v>
       </c>
@@ -82067,7 +82098,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>0.97784414805808939</v>
       </c>
@@ -82108,7 +82139,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>0.96571449717396984</v>
       </c>
@@ -82149,7 +82180,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>0.95977136159576504</v>
       </c>
@@ -82190,7 +82221,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>0.9585237451275026</v>
       </c>
@@ -82231,7 +82262,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>0.9602778582992354</v>
       </c>
@@ -82272,7 +82303,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>0.95871124898397408</v>
       </c>
@@ -82313,7 +82344,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>0.95927223161163733</v>
       </c>
@@ -82354,7 +82385,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>0.96014053153111556</v>
       </c>
@@ -82395,7 +82426,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>0.95775149054888564</v>
       </c>
@@ -82436,7 +82467,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>0.96494711909871478</v>
       </c>
@@ -82477,7 +82508,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>0.95713994499461685</v>
       </c>
@@ -82518,7 +82549,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>0.95577861500109296</v>
       </c>
@@ -82559,7 +82590,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>0.96260971880408619</v>
       </c>
@@ -82600,7 +82631,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>0.95940254177391293</v>
       </c>
@@ -82641,7 +82672,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>0.95577949589101419</v>
       </c>
@@ -82682,7 +82713,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>0.95729069384192467</v>
       </c>
@@ -82723,7 +82754,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>0.95820146443962262</v>
       </c>
@@ -82764,7 +82795,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>0.9583835740335892</v>
       </c>
@@ -82805,7 +82836,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>0.95977388505354155</v>
       </c>
@@ -82846,7 +82877,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>0.95895773129867445</v>
       </c>
@@ -82887,7 +82918,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>0.95902340651899243</v>
       </c>
@@ -82928,7 +82959,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>0.95853028579694377</v>
       </c>
@@ -82969,7 +83000,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>0.9542375752946668</v>
       </c>
@@ -83010,7 +83041,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>0.9425734094107816</v>
       </c>
@@ -83051,7 +83082,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>0.95258634786572349</v>
       </c>
@@ -83092,7 +83123,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>0.96130203904486422</v>
       </c>
@@ -83133,7 +83164,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>0.96819201318969061</v>
       </c>
@@ -83174,7 +83205,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>0.96951897501222728</v>
       </c>
@@ -83215,7 +83246,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>0.96647703466966417</v>
       </c>
@@ -83256,7 +83287,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>0.96820462459615386</v>
       </c>
@@ -83297,7 +83328,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>0.96898670455587577</v>
       </c>
@@ -83338,7 +83369,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>0.96916291872837779</v>
       </c>
@@ -83379,7 +83410,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>0.97402349298655655</v>
       </c>
@@ -83420,7 +83451,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>0.97613944512852124</v>
       </c>
@@ -83461,7 +83492,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>0.98310629702507635</v>
       </c>
@@ -83502,7 +83533,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>0.98685188474469876</v>
       </c>
@@ -83543,7 +83574,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>0.99158427183033215</v>
       </c>
@@ -83584,7 +83615,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>0.99494287940642079</v>
       </c>
@@ -83625,7 +83656,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>1.0117765989346501</v>
       </c>
@@ -83666,7 +83697,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>1.014307553414969</v>
       </c>
@@ -83707,7 +83738,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>1.013836011531186</v>
       </c>
@@ -83748,7 +83779,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>1.0156386917875011</v>
       </c>
@@ -83789,7 +83820,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>1.017786847486633</v>
       </c>
@@ -83830,7 +83861,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>1.018922636989477</v>
       </c>
@@ -83871,7 +83902,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>1.019725567160537</v>
       </c>
@@ -83912,7 +83943,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>1.0215660834656941</v>
       </c>
@@ -83953,7 +83984,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>1.0245360144027711</v>
       </c>
@@ -83994,7 +84025,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>1.027377233660252</v>
       </c>
@@ -84035,7 +84066,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>1.025492093258632</v>
       </c>
@@ -84076,7 +84107,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>1.0311432645495431</v>
       </c>
@@ -84117,7 +84148,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>1.0319625872458349</v>
       </c>
@@ -84158,7 +84189,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>1.033504698878722</v>
       </c>
@@ -84199,7 +84230,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>1.0367619543552731</v>
       </c>
@@ -84240,7 +84271,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>1.038713423771024</v>
       </c>
@@ -84281,7 +84312,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>1.0396734489755519</v>
       </c>
@@ -84322,7 +84353,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>1.0424941775764951</v>
       </c>
@@ -84363,7 +84394,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>1.043846712690732</v>
       </c>
@@ -84404,7 +84435,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>1.045080553779683</v>
       </c>
@@ -86455,6 +86486,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M184" xr:uid="{00000000-0001-0000-0500-000000000000}">
+    <filterColumn colId="12">
+      <filters>
+        <filter val="36_months"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>